<commit_message>
added presentation days for each team
</commit_message>
<xml_diff>
--- a/class resources/2018 - CS 480 - Final Project Presentation Signups.xlsx
+++ b/class resources/2018 - CS 480 - Final Project Presentation Signups.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Day</t>
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>LevidPynch</t>
+  </si>
+  <si>
+    <t>SoundBlaster</t>
+  </si>
+  <si>
+    <t>Team Game Suite</t>
+  </si>
+  <si>
+    <t>Team DTM</t>
+  </si>
+  <si>
+    <t>Greenthumbs</t>
+  </si>
+  <si>
+    <t>Team SNES</t>
+  </si>
+  <si>
+    <t>Dank Spots</t>
+  </si>
+  <si>
+    <t>Cyber Fox Games</t>
+  </si>
+  <si>
+    <t>Speed Daemons</t>
   </si>
 </sst>
 </file>
@@ -343,18 +370,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -362,53 +389,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43220</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43220</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43220</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43220</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43220</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>43222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43222</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43222</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43222</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>43222</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>43222</v>
       </c>
     </row>

</xml_diff>